<commit_message>
terceira questão de pesquisa
</commit_message>
<xml_diff>
--- a/04. Código/causas.xlsx
+++ b/04. Código/causas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,11 +443,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>I.   Algumas doenças infecciosas e parasitárias</t>
+          <t>IX.  Doenças do aparelho circulatório</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>518254</v>
       </c>
     </row>
     <row r="3">
@@ -457,57 +457,57 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1000</v>
+        <v>358364</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>IV.  Doenças endócrinas nutricionais e metabólicas</t>
+          <t>X.   Doenças do aparelho respiratório</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1000</v>
+        <v>204420</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>IX.  Doenças do aparelho circulatório</t>
+          <t>XX.  Causas externas de morbidade e mortalidade</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1000</v>
+        <v>143006</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>IV.  Doenças endócrinas nutricionais e metabólicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1000</v>
+        <v>93801</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>VI.  Doenças do sistema nervoso</t>
+          <t>I.   Algumas doenças infecciosas e parasitárias</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1000</v>
+        <v>92615</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>X.   Doenças do aparelho respiratório</t>
+          <t>XVIII.Sint sinais e achad anorm ex clín e laborat</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1000</v>
+        <v>83448</v>
       </c>
     </row>
     <row r="9">
@@ -517,37 +517,117 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1000</v>
+        <v>80315</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>XIV. Doenças do aparelho geniturinário</t>
+          <t>VI.  Doenças do sistema nervoso</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1000</v>
+        <v>49264</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>XVIII.Sint sinais e achad anorm ex clín e laborat</t>
+          <t>XIV. Doenças do aparelho geniturinário</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1000</v>
+        <v>34486</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>XX.  Causas externas de morbidade e mortalidade</t>
+          <t>V.   Transtornos mentais e comportamentais</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1000</v>
+        <v>13382</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>XIII.Doenças sist osteomuscular e tec conjuntivo</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6616</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>III. Doenças sangue órgãos hemat e transt imunitár</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>6494</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>XII. Doenças da pele e do tecido subcutâneo</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3661</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>XVII.Malf cong deformid e anomalias cromossômicas</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>XV.  Gravidez parto e puerpério</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>XVI. Algumas afec originadas no período perinatal</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>VIII.Doenças do ouvido e da apófise mastóide</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>VII. Doenças do olho e anexos</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>